<commit_message>
only i change left after
</commit_message>
<xml_diff>
--- a/public/downloads/Library of Material Templates.xlsx
+++ b/public/downloads/Library of Material Templates.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noobster\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Template_Name</t>
   </si>
@@ -87,13 +82,73 @@
   </si>
   <si>
     <t>Please don't delete lines 1 to 5 and ensure that only line 6 and below are filled with your templates data. Please avoid adding duplicated templates, duplicated templates will be skiped automaticaly.</t>
+  </si>
+  <si>
+    <t>Field_1_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_2_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_3_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_4_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_5_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_6_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_7_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_8_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_9_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_10_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_11_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_12_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_13_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_14_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_15_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_16_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_17_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_18_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_19_Mandatory</t>
+  </si>
+  <si>
+    <t>Field_20_Mandatory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +309,12 @@
       <family val="2"/>
       <charset val="1"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="34">
@@ -698,8 +759,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -712,9 +782,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -732,6 +799,19 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -800,16 +880,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>537883</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>526676</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>33616</xdr:rowOff>
+      <xdr:rowOff>56028</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>470648</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>459441</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>229435</xdr:rowOff>
+      <xdr:rowOff>251847</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -832,7 +912,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="537883" y="33616"/>
+          <a:off x="1131794" y="56028"/>
           <a:ext cx="1143000" cy="1137113"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -888,7 +968,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -923,7 +1003,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1132,182 +1212,334 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:AO6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:S3"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
+    <row r="1" spans="1:41" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6"/>
+      <c r="AM1" s="6"/>
+      <c r="AN1" s="6"/>
+      <c r="AO1" s="2"/>
     </row>
-    <row r="2" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="6" t="s">
+    <row r="2" spans="1:41" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="2"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="15"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="1"/>
     </row>
-    <row r="3" spans="1:21" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="2"/>
+    <row r="3" spans="1:41" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="12"/>
+      <c r="AA3" s="12"/>
+      <c r="AB3" s="12"/>
+      <c r="AC3" s="12"/>
+      <c r="AD3" s="12"/>
+      <c r="AE3" s="12"/>
+      <c r="AF3" s="12"/>
+      <c r="AG3" s="12"/>
+      <c r="AH3" s="12"/>
+      <c r="AI3" s="12"/>
+      <c r="AJ3" s="13"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="5"/>
+      <c r="AN3" s="5"/>
+      <c r="AO3" s="1"/>
     </row>
-    <row r="4" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
+    <row r="4" spans="1:41" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
+      <c r="AG4" s="7"/>
+      <c r="AH4" s="7"/>
+      <c r="AI4" s="7"/>
+      <c r="AJ4" s="7"/>
+      <c r="AK4" s="7"/>
+      <c r="AL4" s="7"/>
+      <c r="AM4" s="7"/>
+      <c r="AN4" s="7"/>
+      <c r="AO4" s="1"/>
     </row>
-    <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:41" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="G5" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="I5" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="K5" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="M5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="O5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="Q5" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="S5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="T5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="U5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="V5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="W5" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="X5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="Y5" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="AA5" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="AC5" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD5" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="AE5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="AG5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="AI5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="AK5" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="AL5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="AM5" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN5" s="17" t="s">
         <v>20</v>
       </c>
+      <c r="AO5" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="14"/>
     </row>
   </sheetData>
+  <sortState ref="A6:AO9">
+    <sortCondition ref="C6"/>
+  </sortState>
   <mergeCells count="6">
-    <mergeCell ref="T2:U3"/>
-    <mergeCell ref="E1:U1"/>
-    <mergeCell ref="E4:U4"/>
-    <mergeCell ref="A1:D4"/>
-    <mergeCell ref="G2:S3"/>
-    <mergeCell ref="E2:F3"/>
+    <mergeCell ref="AL2:AN3"/>
+    <mergeCell ref="H1:AN1"/>
+    <mergeCell ref="H4:AN4"/>
+    <mergeCell ref="A1:F4"/>
+    <mergeCell ref="L2:AJ3"/>
+    <mergeCell ref="H2:J3"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO1048576 S6:S1048576 U6:U1048576 W6:W1048576 Y6:Y1048576 AA6:AA1048576 AC6:AC1048576 AE6:AE1048576 AG6:AG1048576 AI6:AI1048576 AK6:AK1048576 AM6:AM1048576 Q6:Q1048576 O6:O1048576 M6:M1048576 K6:K1048576 I6:I1048576 G6:G1048576 E6:E1048576 C6:C1048576">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>